<commit_message>
Add the Forest Plot code
</commit_message>
<xml_diff>
--- a/beta_meta_script/input/meta_input.xlsx
+++ b/beta_meta_script/input/meta_input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JLK\AppData\Roaming\MobaXterm\slash\RemoteFiles\394222_2_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JLK\AppData\Roaming\MobaXterm\slash\RemoteFiles\722118_3_23\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -61,9 +61,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>endometriosis</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -73,18 +70,12 @@
     <t>rs10965235</t>
   </si>
   <si>
-    <t>polycystic ovary syndrome</t>
-  </si>
-  <si>
     <t>rs6166</t>
   </si>
   <si>
     <t>G</t>
   </si>
   <si>
-    <t>recurrent spontaneous abortion</t>
-  </si>
-  <si>
     <t>rs1799983</t>
   </si>
   <si>
@@ -98,9 +89,6 @@
   </si>
   <si>
     <t>rs3025039</t>
-  </si>
-  <si>
-    <t>non-obstructive azoospermia</t>
   </si>
   <si>
     <t>rs25487</t>
@@ -132,7 +120,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>oligoasthenoteratozoospermia</t>
+    <t>Endometriosis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Polycystic ovary syndrome</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recurrent spontaneous abortion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oligoasthenoteratozoospermia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Non-obstructive azoospermia</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -518,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -570,16 +574,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -598,16 +602,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -626,16 +630,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -654,16 +658,16 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -682,16 +686,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -710,16 +714,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -738,16 +742,16 @@
     </row>
     <row r="8" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -766,16 +770,16 @@
     </row>
     <row r="9" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -794,16 +798,16 @@
     </row>
     <row r="10" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -822,16 +826,16 @@
     </row>
     <row r="11" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -850,16 +854,16 @@
     </row>
     <row r="12" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -878,16 +882,16 @@
     </row>
     <row r="13" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -906,16 +910,16 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -934,16 +938,16 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -962,16 +966,16 @@
     </row>
     <row r="16" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -990,16 +994,16 @@
     </row>
     <row r="17" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1018,16 +1022,16 @@
     </row>
     <row r="18" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1046,16 +1050,16 @@
     </row>
     <row r="19" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -1074,16 +1078,16 @@
     </row>
     <row r="20" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -1102,16 +1106,16 @@
     </row>
     <row r="21" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -1130,16 +1134,16 @@
     </row>
     <row r="22" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1158,16 +1162,16 @@
     </row>
     <row r="23" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -1186,16 +1190,16 @@
     </row>
     <row r="24" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -1214,16 +1218,16 @@
     </row>
     <row r="25" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -1242,16 +1246,16 @@
     </row>
     <row r="26" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -1270,16 +1274,16 @@
     </row>
     <row r="27" spans="1:10" ht="27.6" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>

</xml_diff>